<commit_message>
corrected typos in earnings excel
</commit_message>
<xml_diff>
--- a/earnings_page.xlsx
+++ b/earnings_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ft/Documents/Tecky/stonks2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FC75C20-570C-4348-AACE-E4EE988AD15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E39538-9E52-B144-9208-6B5790AC42FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{951900C3-487F-AE42-8EE1-A20C6DC3A600}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="History_Prnt">[1]SENTIMENT!$A$2:$G$1987,[1]SENTIMENT!$K$2:$M$313</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -127,9 +127,6 @@
     <t>Costco Wholesale Corp</t>
   </si>
   <si>
-    <t>Up-coming Earnings Realses in the coming 10 days:</t>
-  </si>
-  <si>
     <t>FDX</t>
   </si>
   <si>
@@ -182,6 +179,9 @@
   </si>
   <si>
     <t>Factset Research Sys Inc</t>
+  </si>
+  <si>
+    <t>Up-coming Earnings Releases in the coming 10 days:</t>
   </si>
 </sst>
 </file>
@@ -47972,7 +47972,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B1ADE9-ADE1-5840-B17D-6B761B3CAEB1}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <cols>
@@ -48851,7 +48853,7 @@
     </row>
     <row r="17" spans="1:11" ht="15">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -48894,10 +48896,10 @@
         <v>44637</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20">
         <v>2022</v>
@@ -48919,10 +48921,10 @@
         <v>44637</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21">
         <v>2022</v>
@@ -48944,10 +48946,10 @@
         <v>44637</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>2021</v>
@@ -48969,10 +48971,10 @@
         <v>44641</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23">
         <v>2022</v>
@@ -48994,10 +48996,10 @@
         <v>44642</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24">
         <v>2022</v>
@@ -49019,10 +49021,10 @@
         <v>44643</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25">
         <v>2022</v>
@@ -49044,10 +49046,10 @@
         <v>44643</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <v>2022</v>
@@ -49069,10 +49071,10 @@
         <v>44644</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27">
         <v>2022</v>
@@ -49092,10 +49094,10 @@
         <v>44644</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28">
         <v>2022</v>

</xml_diff>